<commit_message>
Inital board & bunch of schematic changes
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewforsman/Practicum/synthy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bridge/Git/synthy/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -84,13 +81,34 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>1993-1066-ND</t>
+  </si>
+  <si>
+    <t>PT10MV10-103A2020-E-S</t>
+  </si>
+  <si>
+    <t>Unit price</t>
+  </si>
+  <si>
+    <t>POT 10K OHM LINEAR</t>
+  </si>
+  <si>
+    <t>BFC280800006</t>
+  </si>
+  <si>
+    <t> Components</t>
+  </si>
+  <si>
+    <t>CAP TRIMMER 2.5-22PF 250V TH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,6 +128,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,11 +156,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -416,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,10 +451,12 @@
     <col min="1" max="1" width="41.5" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" customWidth="1"/>
     <col min="3" max="3" width="28.83203125" customWidth="1"/>
-    <col min="6" max="6" width="33.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,16 +467,19 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -460,14 +489,18 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
+        <v>8.94</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
+        <f>E2*D2</f>
         <v>8.94</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -478,13 +511,17 @@
         <v>10</v>
       </c>
       <c r="D3">
+        <v>1.41</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F7" si="0">E3*D3</f>
         <v>1.41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -495,13 +532,17 @@
         <v>13</v>
       </c>
       <c r="D4">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -509,27 +550,77 @@
         <v>15</v>
       </c>
       <c r="D5">
+        <v>6.58</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
         <v>6.58</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D40" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>0.49</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>2.89</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
         <v>18</v>
       </c>
-      <c r="E40">
-        <f>SUM(E2:E38)</f>
-        <v>18.07</v>
+      <c r="F40">
+        <f>SUM(F2:F38)</f>
+        <v>25.810000000000002</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C7" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>